<commit_message>
Abstract and Introduction Complete
</commit_message>
<xml_diff>
--- a/Labs/Lab 5 - Electron Diffraction/data.xlsx
+++ b/Labs/Lab 5 - Electron Diffraction/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7DF0A3-CD63-461E-A67E-17FE4B6F8B19}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3400452E-3AA9-4141-87D3-73602D735A18}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>Voltage</t>
   </si>
@@ -169,6 +169,24 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   </t>
+  </si>
+  <si>
+    <t>max gradient</t>
+  </si>
+  <si>
+    <t>min gradient</t>
+  </si>
+  <si>
+    <t>+/- 9.1%</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -253,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -261,13 +279,18 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -891,6 +914,32 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -921,6 +970,44 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'Data attempt 2'!$E$3:$E$12</c:f>
@@ -1070,6 +1157,44 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'Data attempt 2'!$E$20:$E$29</c:f>
@@ -1152,6 +1277,210 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C72F-438D-970A-CB01195568DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>maxInner</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.20275614552605703"/>
+                  <c:y val="-6.1131020659542956E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data attempt 2'!$J$32:$J$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>30.911999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.508499999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data attempt 2'!$I$32:$I$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.7407765595569783E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2909944487358056E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4E11-4C9E-BE60-CDF7CE23060C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>minInner</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data attempt 2'!$K$32:$K$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>27.967999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.351500000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data attempt 2'!$I$32:$I$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.7407765595569783E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2909944487358056E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4E11-4C9E-BE60-CDF7CE23060C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2640,16 +2969,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>580501</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>27233</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>11351</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>127612</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2963,12 +3292,12 @@
       <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
@@ -3257,12 +3586,12 @@
       <c r="B19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
@@ -3555,13 +3884,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F2AD85-DFC9-4D18-B96E-927328BE276B}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="11" width="14.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -3570,12 +3902,12 @@
       <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3845,25 +4177,25 @@
       <c r="B16" s="6"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
         <v>1</v>
@@ -3878,7 +4210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3300</v>
       </c>
@@ -3901,7 +4233,7 @@
         <v>7.5949367088607627</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3600</v>
       </c>
@@ -3924,7 +4256,7 @@
         <v>7.8242229367631273</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>3900</v>
       </c>
@@ -3947,7 +4279,7 @@
         <v>6.66966090276218</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>4200</v>
       </c>
@@ -3970,7 +4302,7 @@
         <v>3.5911602209944804</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4500</v>
       </c>
@@ -3993,7 +4325,7 @@
         <v>6.561808798230528</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>4800</v>
       </c>
@@ -4016,7 +4348,7 @@
         <v>5.8038007190549701</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>5100</v>
       </c>
@@ -4039,7 +4371,7 @@
         <v>5.4018445322793065</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>5500</v>
       </c>
@@ -4062,7 +4394,7 @@
         <v>6.2200956937799061</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>5700</v>
       </c>
@@ -4085,7 +4417,7 @@
         <v>6.9436539556061394</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>6000</v>
       </c>
@@ -4108,7 +4440,7 @@
         <v>5.7983942908117845</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="F30" s="3">
         <f>SUM(F20:F29)/10</f>
@@ -4117,15 +4449,90 @@
       <c r="G30" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="J30" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J31" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G32" s="11"/>
+      <c r="I32" s="6">
+        <v>1.7407765595569783E-2</v>
+      </c>
+      <c r="J32">
+        <f>1.05*E3</f>
+        <v>30.911999999999999</v>
+      </c>
+      <c r="K32">
+        <f>0.95*E3</f>
+        <v>27.967999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I33" s="6">
+        <v>1.2909944487358056E-2</v>
+      </c>
+      <c r="J33">
+        <f>0.95*E12</f>
+        <v>17.508499999999998</v>
+      </c>
+      <c r="K33">
+        <f>1.05*E12</f>
+        <v>19.351500000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="J35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="10"/>
+    </row>
+    <row r="36" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="J36" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I37" s="6">
+        <v>1.7407765595569783E-2</v>
+      </c>
+      <c r="J37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I38" s="6">
+        <v>1.2909944487358056E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J35:K35"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4134,7 +4541,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4174,9 +4581,8 @@
         <f>B2*(1000)</f>
         <v>0.6</v>
       </c>
-      <c r="C3">
-        <f>C2*(1000)</f>
-        <v>0.4</v>
+      <c r="C3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4188,18 +4594,17 @@
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6">
-        <f>(m_1*L)/(SQRT((e*m)/(2*h^2)))</f>
-        <v>2.0604176955011781E-10</v>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="e">
         <f>(m_2*L)/SQRT((e*m)/(2*h^2))</f>
-        <v>1.3736117970007857E-10</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4238,7 +4643,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
+      <c r="B14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>